<commit_message>
add query gap to ini file and add save to pgsql
</commit_message>
<xml_diff>
--- a/第五医院信息表.xlsx
+++ b/第五医院信息表.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="150">
   <si>
     <t>科室</t>
   </si>
@@ -36,16 +36,25 @@
     <t>杨芳</t>
   </si>
   <si>
-    <t>本周六07/01[0];</t>
-  </si>
-  <si>
-    <t>下周六07/08[35];下周二07/04[35];</t>
+    <t>本周二07/04[34];本周六07/08[34];</t>
   </si>
   <si>
     <t>陈芳莲</t>
   </si>
   <si>
-    <t>下周五07/07[30];下周一07/03[33];</t>
+    <t>本周五07/07[29];</t>
+  </si>
+  <si>
+    <t>下周一07/10[35];</t>
+  </si>
+  <si>
+    <t>儿科门诊</t>
+  </si>
+  <si>
+    <t>黄教</t>
+  </si>
+  <si>
+    <t>本周二07/04[35];本周六07/08[35];</t>
   </si>
   <si>
     <t>泌尿外科门诊</t>
@@ -54,13 +63,16 @@
     <t>肖继光</t>
   </si>
   <si>
-    <t>下周五07/07[35];下周二07/04[35];</t>
+    <t>本周二07/04[35];本周五07/07[35];</t>
   </si>
   <si>
     <t>崔晓洁</t>
   </si>
   <si>
-    <t>下周一07/03[26];下周四07/06[33];</t>
+    <t>本周一07/03[25];本周四07/06[31];</t>
+  </si>
+  <si>
+    <t>下周一07/10[30];</t>
   </si>
   <si>
     <t>消化内科门诊</t>
@@ -69,7 +81,10 @@
     <t>周东生</t>
   </si>
   <si>
-    <t>下周一07/03[41];下周四07/06[35];</t>
+    <t>本周四07/06[35];</t>
+  </si>
+  <si>
+    <t>下周一07/10[43];</t>
   </si>
   <si>
     <t>外科门诊</t>
@@ -78,7 +93,31 @@
     <t>张宪国</t>
   </si>
   <si>
-    <t>下周五07/07[35];下周一07/03[34];</t>
+    <t>本周五07/07[35];</t>
+  </si>
+  <si>
+    <t>骨二科门诊</t>
+  </si>
+  <si>
+    <t>陆凌云</t>
+  </si>
+  <si>
+    <t>本周一07/03[30];</t>
+  </si>
+  <si>
+    <t>下周一07/10[65];</t>
+  </si>
+  <si>
+    <t>内分泌科门诊</t>
+  </si>
+  <si>
+    <t>冯尤健</t>
+  </si>
+  <si>
+    <t>本周四07/06[42];</t>
+  </si>
+  <si>
+    <t>下周一07/10[42];</t>
   </si>
   <si>
     <t>骨一科门诊</t>
@@ -87,61 +126,49 @@
     <t>陈学飞</t>
   </si>
   <si>
-    <t>下周五07/07[35];</t>
-  </si>
-  <si>
-    <t>骨二科门诊</t>
-  </si>
-  <si>
-    <t>陆凌云</t>
-  </si>
-  <si>
-    <t>下周一07/03[65];</t>
-  </si>
-  <si>
-    <t>内分泌科门诊</t>
-  </si>
-  <si>
-    <t>冯尤健</t>
-  </si>
-  <si>
-    <t>下周四07/06[42];下周一07/03[41];</t>
-  </si>
-  <si>
-    <t>儿科门诊</t>
+    <t>刘汉昌</t>
+  </si>
+  <si>
+    <t>本周四07/06[34];</t>
+  </si>
+  <si>
+    <t>舒诗军</t>
+  </si>
+  <si>
+    <t>本周六07/08[35];</t>
+  </si>
+  <si>
+    <t>池晓蓉</t>
+  </si>
+  <si>
+    <t>本周五07/07[34];</t>
+  </si>
+  <si>
+    <t>耳鼻喉科门诊</t>
+  </si>
+  <si>
+    <t>刘海楼</t>
   </si>
   <si>
     <t>姜敏</t>
   </si>
   <si>
-    <t>池晓蓉</t>
-  </si>
-  <si>
-    <t>耳鼻喉科门诊</t>
-  </si>
-  <si>
-    <t>刘海楼</t>
-  </si>
-  <si>
-    <t>下周四07/06[34];下周一07/03[34];</t>
+    <t>陈魁夫</t>
+  </si>
+  <si>
+    <t>本周六07/08[35];本周三07/05[34];</t>
   </si>
   <si>
     <t>洪海填</t>
   </si>
   <si>
-    <t>下周二07/04[35];下周五07/07[35];</t>
-  </si>
-  <si>
-    <t>刘汉昌</t>
-  </si>
-  <si>
-    <t>下周四07/06[35];下周一07/03[34];</t>
+    <t>本周五07/07[35];本周二07/04[35];</t>
   </si>
   <si>
     <t>朱上敏</t>
   </si>
   <si>
-    <t>下周三07/05[35];下周一07/03[33];</t>
+    <t>本周三07/05[35];</t>
   </si>
   <si>
     <t>产科门诊</t>
@@ -150,28 +177,28 @@
     <t>张金香</t>
   </si>
   <si>
-    <t>下周一07/03[13];</t>
-  </si>
-  <si>
-    <t>黄教</t>
-  </si>
-  <si>
-    <t>下周二07/04[35];下周六07/08[35];</t>
+    <t>本周一07/03[0];</t>
+  </si>
+  <si>
+    <t>下周一07/10[27];</t>
+  </si>
+  <si>
+    <t>眼科门诊</t>
+  </si>
+  <si>
+    <t>陈胡挪</t>
+  </si>
+  <si>
+    <t>李春阳</t>
+  </si>
+  <si>
+    <t>本周六07/08[35];本周四07/06[35];</t>
   </si>
   <si>
     <t>洪山</t>
   </si>
   <si>
-    <t>下周四07/06[35];下周一07/03[30];</t>
-  </si>
-  <si>
-    <t>眼科门诊</t>
-  </si>
-  <si>
-    <t>陈胡挪</t>
-  </si>
-  <si>
-    <t>下周一07/03[34];下周四07/06[35];</t>
+    <t>本周一07/03[27];本周四07/06[35];</t>
   </si>
   <si>
     <t>心血管内科门诊</t>
@@ -180,88 +207,79 @@
     <t>李勇胜</t>
   </si>
   <si>
-    <t>下周四07/06[65];</t>
+    <t>本周四07/06[64];</t>
   </si>
   <si>
     <t>神经内科门诊</t>
   </si>
   <si>
+    <t>张辉</t>
+  </si>
+  <si>
     <t>梁富龙</t>
   </si>
   <si>
-    <t>张辉</t>
-  </si>
-  <si>
-    <t>下周四07/06[35];下周一07/03[35];</t>
-  </si>
-  <si>
-    <t>李春阳</t>
-  </si>
-  <si>
-    <t>下周四07/06[35];下周六07/08[35];</t>
-  </si>
-  <si>
-    <t>舒诗军</t>
-  </si>
-  <si>
-    <t>下周六07/08[35];</t>
+    <t>吴谨准</t>
+  </si>
+  <si>
+    <t>本周二07/04[6];</t>
+  </si>
+  <si>
+    <t>中医科门诊</t>
+  </si>
+  <si>
+    <t>苏炳伟</t>
+  </si>
+  <si>
+    <t>本周六07/08[35];本周二07/04[35];</t>
+  </si>
+  <si>
+    <t>张燕</t>
+  </si>
+  <si>
+    <t>本周三07/05[18];</t>
   </si>
   <si>
     <t>战晟</t>
   </si>
   <si>
-    <t>下周四07/06[35];</t>
-  </si>
-  <si>
-    <t>吴谨准</t>
-  </si>
-  <si>
-    <t>下周二07/04[9];</t>
-  </si>
-  <si>
-    <t>张燕</t>
-  </si>
-  <si>
-    <t>下周三07/05[18];</t>
-  </si>
-  <si>
-    <t>陈魁夫</t>
-  </si>
-  <si>
-    <t>下周六07/08[35];下周三07/05[35];</t>
-  </si>
-  <si>
     <t>呼吸内科门诊</t>
   </si>
   <si>
     <t>邹良能</t>
   </si>
   <si>
-    <t>下周三07/05[35];下周一07/03[35];</t>
-  </si>
-  <si>
     <t>肾病风湿免疫科门诊</t>
   </si>
   <si>
+    <t>林鹰</t>
+  </si>
+  <si>
+    <t>盛群英</t>
+  </si>
+  <si>
+    <t>本周五07/07[30];本周三07/05[27];</t>
+  </si>
+  <si>
     <t>钟鸿斌</t>
   </si>
   <si>
-    <t>下周三07/05[35];下周五07/07[35];</t>
-  </si>
-  <si>
-    <t>盛群英</t>
-  </si>
-  <si>
-    <t>下周五07/07[30];下周三07/05[28];</t>
+    <t>本周三07/05[35];本周五07/07[35];</t>
+  </si>
+  <si>
+    <t>傅翔</t>
   </si>
   <si>
     <t>风湿免疫科门诊</t>
   </si>
   <si>
-    <t>中医科门诊</t>
-  </si>
-  <si>
-    <t>苏炳伟</t>
+    <t>本周五07/07[35];本周三07/05[35];</t>
+  </si>
+  <si>
+    <t>心血管内科专家门诊</t>
+  </si>
+  <si>
+    <t>谢强</t>
   </si>
   <si>
     <t>肿瘤内科门诊</t>
@@ -270,22 +288,28 @@
     <t>傅鉴乾</t>
   </si>
   <si>
+    <t>感染性疾病科门诊</t>
+  </si>
+  <si>
+    <t>薛秀兰</t>
+  </si>
+  <si>
+    <t>本周二07/04[28];</t>
+  </si>
+  <si>
     <t>康复医学科门诊</t>
   </si>
   <si>
     <t>郑丁炤</t>
   </si>
   <si>
-    <t>下周一07/03[35];下周三07/05[35];</t>
-  </si>
-  <si>
     <t>胸心外科门诊</t>
   </si>
   <si>
     <t>贾平</t>
   </si>
   <si>
-    <t>下周二07/04[35];下周四07/06[35];</t>
+    <t>本周四07/06[35];本周二07/04[35];</t>
   </si>
   <si>
     <t>心血管外科专家门诊</t>
@@ -294,19 +318,16 @@
     <t>林乌拉</t>
   </si>
   <si>
-    <t>下周六07/08[30];</t>
+    <t>本周六07/08[30];</t>
   </si>
   <si>
     <t>李泰标</t>
   </si>
   <si>
-    <t>感染性疾病科门诊</t>
-  </si>
-  <si>
-    <t>薛秀兰</t>
-  </si>
-  <si>
-    <t>下周二07/04[29];</t>
+    <t>陈永春</t>
+  </si>
+  <si>
+    <t>本周二07/04[35];</t>
   </si>
   <si>
     <t>神经外科门诊</t>
@@ -315,24 +336,15 @@
     <t>专家号</t>
   </si>
   <si>
-    <t>本周日07/02[78];</t>
-  </si>
-  <si>
-    <t>下周三07/05[35];下周五07/07[78];下周二07/04[78];下周六07/08[78];下周四07/06[78];下周一07/03[78];</t>
+    <t>本周六07/08[78];本周四07/06[78];本周一07/03[36];本周二07/04[78];本周五07/07[78];本周日07/09[78];本周三07/05[35];</t>
+  </si>
+  <si>
+    <t>下周一07/10[78];</t>
   </si>
   <si>
     <t>神经内科</t>
   </si>
   <si>
-    <t>林鹰</t>
-  </si>
-  <si>
-    <t>陈永春</t>
-  </si>
-  <si>
-    <t>下周二07/04[35];</t>
-  </si>
-  <si>
     <t>张芸</t>
   </si>
   <si>
@@ -345,19 +357,16 @@
     <t>普通号</t>
   </si>
   <si>
-    <t>本周日07/02[77];</t>
-  </si>
-  <si>
-    <t>下周二07/04[78];下周五07/07[78];下周三07/05[78];下周六07/08[78];下周一07/03[78];下周四07/06[78];</t>
+    <t>本周六07/08[78];本周二07/04[78];本周五07/07[78];本周一07/03[35];本周日07/09[78];本周三07/05[78];本周四07/06[78];</t>
   </si>
   <si>
     <t>全科医学科门诊</t>
   </si>
   <si>
-    <t>下周三07/05[78];下周六07/08[78];下周一07/03[78];下周四07/06[78];下周二07/04[78];下周五07/07[78];</t>
-  </si>
-  <si>
-    <t>下周六07/08[78];下周一07/03[78];下周四07/06[78];下周二07/04[78];下周五07/07[78];下周三07/05[78];</t>
+    <t>本周二07/04[78];本周五07/07[78];本周一07/03[35];本周日07/09[78];本周三07/05[78];本周四07/06[78];本周六07/08[78];</t>
+  </si>
+  <si>
+    <t>本周日07/09[78];本周三07/05[78];本周四07/06[78];本周六07/08[78];本周二07/04[78];本周五07/07[78];本周一07/03[35];</t>
   </si>
   <si>
     <t>老年病科</t>
@@ -366,19 +375,22 @@
     <t>介入诊疗科门诊</t>
   </si>
   <si>
-    <t>下周六07/08[78];下周四07/06[78];下周一07/03[78];下周三07/05[35];下周五07/07[78];下周二07/04[78];</t>
-  </si>
-  <si>
-    <t>下周五07/07[78];下周三07/05[78];下周六07/08[78];下周一07/03[78];下周四07/06[78];下周二07/04[78];</t>
-  </si>
-  <si>
-    <t>下周二07/04[78];下周五07/07[78];下周三07/05[78];下周六07/08[78];下周四07/06[78];下周一07/03[78];</t>
-  </si>
-  <si>
-    <t>下周二07/04[78];下周六07/08[78];下周一07/03[78];下周四07/06[78];下周三07/05[35];下周五07/07[78];</t>
-  </si>
-  <si>
-    <t>下周六07/08[78];下周四07/06[78];下周一07/03[78];下周二07/04[78];下周五07/07[78];下周三07/05[78];</t>
+    <t>本周日07/09[78];本周三07/05[35];本周六07/08[78];本周四07/06[78];本周一07/03[36];本周二07/04[78];本周五07/07[78];</t>
+  </si>
+  <si>
+    <t>本周三07/05[78];本周四07/06[78];本周六07/08[78];本周二07/04[78];本周五07/07[78];本周一07/03[35];本周日07/09[78];</t>
+  </si>
+  <si>
+    <t>本周四07/06[78];本周一07/03[36];本周二07/04[78];本周五07/07[78];本周日07/09[78];本周三07/05[35];本周六07/08[78];</t>
+  </si>
+  <si>
+    <t>本周三07/05[35];本周六07/08[78];本周四07/06[78];本周一07/03[36];本周二07/04[78];本周五07/07[78];本周日07/09[78];</t>
+  </si>
+  <si>
+    <t>本周四07/06[78];本周六07/08[78];本周二07/04[78];本周五07/07[78];本周一07/03[35];本周日07/09[78];本周三07/05[78];</t>
+  </si>
+  <si>
+    <t>本周日07/09[78];本周三07/05[78];本周四07/06[78];本周六07/08[78];本周五07/07[78];本周二07/04[78];本周一07/03[35];</t>
   </si>
   <si>
     <t>中医皮肤科</t>
@@ -387,49 +399,31 @@
     <t>肛肠科门诊</t>
   </si>
   <si>
-    <t>下周一07/03[78];下周四07/06[78];下周二07/04[78];下周五07/07[78];下周三07/05[78];下周六07/08[78];</t>
-  </si>
-  <si>
     <t>皮肤科</t>
   </si>
   <si>
-    <t>下周三07/05[78];下周六07/08[78];下周四07/06[78];下周一07/03[78];下周二07/04[78];下周五07/07[78];</t>
-  </si>
-  <si>
     <t>朱冰封</t>
   </si>
   <si>
-    <t>下周三07/05[35];</t>
-  </si>
-  <si>
-    <t>傅翔</t>
-  </si>
-  <si>
     <t>单忠贵</t>
   </si>
   <si>
     <t>陈佳山</t>
   </si>
   <si>
-    <t>下周二07/04[35];下周三07/05[35];</t>
+    <t>本周三07/05[35];本周二07/04[35];</t>
   </si>
   <si>
     <t>文鉴立</t>
   </si>
   <si>
-    <t>下周一07/03[35];下周四07/06[35];</t>
-  </si>
-  <si>
     <t>鲁丛霞</t>
   </si>
   <si>
-    <t>心血管内科专家门诊</t>
-  </si>
-  <si>
     <t>吴荣</t>
   </si>
   <si>
-    <t>下周三07/05[20];</t>
+    <t>本周三07/05[20];</t>
   </si>
   <si>
     <t>肾内科专家门诊</t>
@@ -438,7 +432,7 @@
     <t>黄继义</t>
   </si>
   <si>
-    <t>下周一07/03[6];</t>
+    <t>下周一07/10[6];</t>
   </si>
   <si>
     <t>白海涛</t>
@@ -453,7 +447,7 @@
     <t>曹本福</t>
   </si>
   <si>
-    <t>下周二07/04[65];</t>
+    <t>本周二07/04[65];</t>
   </si>
   <si>
     <t>柳滨</t>
@@ -462,7 +456,7 @@
     <t>万会来</t>
   </si>
   <si>
-    <t>下周二07/04[64];</t>
+    <t>本周二07/04[63];</t>
   </si>
   <si>
     <t>消化内科二科</t>
@@ -471,7 +465,7 @@
     <t>张志阳</t>
   </si>
   <si>
-    <t>下周四07/06[30];</t>
+    <t>本周四07/06[30];</t>
   </si>
 </sst>
 </file>
@@ -841,7 +835,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D94"/>
+  <dimension ref="A1:D95"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -879,18 +873,18 @@
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="D2" s="1" t="s"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1" t="s"/>
       <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
@@ -902,583 +896,597 @@
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1" t="s"/>
-      <c r="D4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="D4" s="1" t="s"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="1" t="s"/>
-      <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1" t="s"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="1" t="s"/>
+      <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="D6" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="1" t="s"/>
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="D7" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="1" t="s"/>
+        <v>24</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="D8" s="1" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="1" t="s"/>
+        <v>27</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="D9" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="1" t="s"/>
+        <v>31</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="D10" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="1" t="s"/>
-      <c r="D11" s="1" t="s">
-        <v>23</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="1" t="s"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="1" t="s"/>
+        <v>36</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="D12" s="1" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="1" t="s"/>
-      <c r="D13" s="1" t="s">
-        <v>35</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="1" t="s"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="1" t="s"/>
-      <c r="D14" s="1" t="s">
-        <v>37</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="1" t="s"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="1" t="s"/>
+        <v>43</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="D15" s="1" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="1" t="s"/>
-      <c r="D16" s="1" t="s">
-        <v>41</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="1" t="s"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="1" t="s"/>
-      <c r="D17" s="1" t="s">
-        <v>44</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="1" t="s"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>46</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="D18" s="1" t="s"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" s="1" t="s"/>
+        <v>49</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="D19" s="1" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C20" s="1" t="s"/>
+        <v>52</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="D20" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" s="1" t="s"/>
+        <v>56</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="D21" s="1" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" s="1" t="s"/>
-      <c r="D22" s="1" t="s">
-        <v>37</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" s="1" t="s"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C23" s="1" t="s"/>
+        <v>59</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="D23" s="1" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>18</v>
+        <v>61</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>60</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="D24" s="1" t="s"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="D25" s="1" t="s">
-        <v>62</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C26" s="1" t="s"/>
-      <c r="D26" s="1" t="s">
-        <v>64</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="1" t="s"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C27" s="1" t="s"/>
-      <c r="D27" s="1" t="s">
-        <v>66</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" s="1" t="s"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C28" s="1" t="s"/>
-      <c r="D28" s="1" t="s">
-        <v>68</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" s="1" t="s"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>70</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="D29" s="1" t="s"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C30" s="1" t="s"/>
-      <c r="D30" s="1" t="s">
-        <v>73</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" s="1" t="s"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C31" s="1" t="s"/>
+        <v>76</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="D31" s="1" t="s">
-        <v>76</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>4</v>
+        <v>77</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C32" s="1" t="s"/>
-      <c r="D32" s="1" t="s">
         <v>78</v>
       </c>
+      <c r="C32" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D32" s="1" t="s"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C33" s="1" t="s"/>
-      <c r="D33" s="1" t="s">
-        <v>76</v>
-      </c>
+      <c r="C33" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D33" s="1" t="s"/>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>81</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>7</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="D34" s="1" t="s"/>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C35" s="1" t="s"/>
-      <c r="D35" s="1" t="s">
-        <v>58</v>
-      </c>
+      <c r="C35" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D35" s="1" t="s"/>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C36" s="1" t="s"/>
-      <c r="D36" s="1" t="s">
-        <v>86</v>
-      </c>
+      <c r="D36" s="1" t="s"/>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="C37" s="1" t="s"/>
       <c r="D37" s="1" t="s">
-        <v>89</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C38" s="1" t="s"/>
+        <v>89</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="D38" s="1" t="s">
-        <v>92</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C39" s="1" t="s"/>
-      <c r="D39" s="1" t="s">
-        <v>37</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D39" s="1" t="s"/>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C40" s="1" t="s"/>
+      <c r="C40" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="D40" s="1" t="s">
-        <v>96</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>100</v>
-      </c>
+      <c r="D41" s="1" t="s"/>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C42" s="1" t="s"/>
-      <c r="D42" s="1" t="s">
-        <v>37</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D42" s="1" t="s"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>46</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D43" s="1" t="s"/>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C44" s="1" t="s"/>
-      <c r="D44" s="1" t="s">
-        <v>104</v>
-      </c>
+      <c r="D44" s="1" t="s"/>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C45" s="1" t="s"/>
+      <c r="C45" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="D45" s="1" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C46" s="1" t="s"/>
-      <c r="D46" s="1" t="s">
-        <v>26</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D46" s="1" t="s"/>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>108</v>
+        <v>78</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>110</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="D47" s="1" t="s"/>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>112</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="D48" s="1" t="s"/>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>109</v>
+        <v>28</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>110</v>
+        <v>29</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>79</v>
+        <v>111</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="51">
@@ -1486,588 +1494,604 @@
         <v>114</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="D52" s="1" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>115</v>
+        <v>84</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>74</v>
+        <v>117</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>52</v>
+        <v>118</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>55</v>
+        <v>118</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="s">
-        <v>122</v>
+        <v>19</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
-        <v>94</v>
+        <v>13</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="s">
-        <v>80</v>
+        <v>125</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="s">
-        <v>21</v>
+        <v>127</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="s">
-        <v>84</v>
+        <v>34</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>99</v>
+        <v>120</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="s">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="s">
-        <v>33</v>
+        <v>93</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="s">
-        <v>97</v>
+        <v>55</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C78" s="1" t="s"/>
+        <v>112</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="D78" s="1" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>6</v>
+        <v>116</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>7</v>
+        <v>107</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="s">
-        <v>87</v>
+        <v>23</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C80" s="1" t="s"/>
+        <v>112</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="D80" s="1" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="s">
-        <v>114</v>
+        <v>10</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C81" s="1" t="s"/>
-      <c r="D81" s="1" t="s">
-        <v>131</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D81" s="1" t="s"/>
     </row>
     <row r="82">
       <c r="A82" s="1" t="s">
-        <v>74</v>
+        <v>114</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>7</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="D82" s="1" t="s"/>
     </row>
     <row r="83">
       <c r="A83" s="1" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C83" s="1" t="s"/>
-      <c r="D83" s="1" t="s">
-        <v>133</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D83" s="1" t="s"/>
     </row>
     <row r="84">
       <c r="A84" s="1" t="s">
-        <v>55</v>
+        <v>117</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C84" s="1" t="s"/>
-      <c r="D84" s="1" t="s">
-        <v>127</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D84" s="1" t="s"/>
     </row>
     <row r="85">
       <c r="A85" s="1" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="s">
-        <v>135</v>
+        <v>64</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C86" s="1" t="s"/>
-      <c r="D86" s="1" t="s">
-        <v>137</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D86" s="1" t="s"/>
     </row>
     <row r="87">
       <c r="A87" s="1" t="s">
-        <v>138</v>
+        <v>86</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C87" s="1" t="s"/>
-      <c r="D87" s="1" t="s">
-        <v>140</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D87" s="1" t="s"/>
     </row>
     <row r="88">
       <c r="A88" s="1" t="s">
-        <v>30</v>
+        <v>136</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C88" s="1" t="s"/>
+        <v>137</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="D88" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C89" s="1" t="s"/>
-      <c r="D89" s="1" t="s">
-        <v>127</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D89" s="1" t="s"/>
     </row>
     <row r="90">
       <c r="A90" s="1" t="s">
-        <v>97</v>
+        <v>26</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C90" s="1" t="s"/>
-      <c r="D90" s="1" t="s">
-        <v>127</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D90" s="1" t="s"/>
     </row>
     <row r="91">
       <c r="A91" s="1" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C91" s="1" t="s"/>
-      <c r="D91" s="1" t="s">
-        <v>145</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D91" s="1" t="s"/>
     </row>
     <row r="92">
       <c r="A92" s="1" t="s">
-        <v>18</v>
+        <v>104</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C92" s="1" t="s"/>
-      <c r="D92" s="1" t="s">
-        <v>127</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D92" s="1" t="s"/>
     </row>
     <row r="93">
       <c r="A93" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C93" s="1" t="s"/>
-      <c r="D93" s="1" t="s">
-        <v>148</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D93" s="1" t="s"/>
     </row>
     <row r="94">
       <c r="A94" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D94" s="1" t="s"/>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C95" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B94" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C94" s="1" t="s"/>
-      <c r="D94" s="1" t="s">
-        <v>151</v>
-      </c>
+      <c r="D95" s="1" t="s"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
add inorupdate to pgsql
</commit_message>
<xml_diff>
--- a/第五医院信息表.xlsx
+++ b/第五医院信息表.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="157">
   <si>
     <t>科室</t>
   </si>
@@ -36,7 +36,10 @@
     <t>杨芳</t>
   </si>
   <si>
-    <t>本周二07/04[34];本周六07/08[34];</t>
+    <t>本周六07/08[32];</t>
+  </si>
+  <si>
+    <t>下周二07/11[34];</t>
   </si>
   <si>
     <t>陈芳莲</t>
@@ -45,109 +48,154 @@
     <t>本周五07/07[29];</t>
   </si>
   <si>
+    <t>下周一07/10[34];</t>
+  </si>
+  <si>
+    <t>儿科门诊</t>
+  </si>
+  <si>
+    <t>黄教</t>
+  </si>
+  <si>
+    <t>本周六07/08[35];</t>
+  </si>
+  <si>
+    <t>下周二07/11[50];</t>
+  </si>
+  <si>
+    <t>消化内科门诊</t>
+  </si>
+  <si>
+    <t>周东生</t>
+  </si>
+  <si>
+    <t>本周四07/06[35];</t>
+  </si>
+  <si>
+    <t>下周一07/10[43];</t>
+  </si>
+  <si>
+    <t>崔晓洁</t>
+  </si>
+  <si>
+    <t>本周四07/06[29];</t>
+  </si>
+  <si>
+    <t>下周一07/10[29];</t>
+  </si>
+  <si>
+    <t>泌尿外科门诊</t>
+  </si>
+  <si>
+    <t>肖继光</t>
+  </si>
+  <si>
+    <t>本周五07/07[35];</t>
+  </si>
+  <si>
+    <t>下周二07/11[35];</t>
+  </si>
+  <si>
+    <t>骨二科门诊</t>
+  </si>
+  <si>
+    <t>陆凌云</t>
+  </si>
+  <si>
+    <t>下周一07/10[65];</t>
+  </si>
+  <si>
+    <t>耳鼻喉科门诊</t>
+  </si>
+  <si>
+    <t>刘海楼</t>
+  </si>
+  <si>
+    <t>本周四07/06[34];</t>
+  </si>
+  <si>
     <t>下周一07/10[35];</t>
   </si>
   <si>
-    <t>儿科门诊</t>
-  </si>
-  <si>
-    <t>黄教</t>
-  </si>
-  <si>
-    <t>本周二07/04[35];本周六07/08[35];</t>
-  </si>
-  <si>
-    <t>泌尿外科门诊</t>
-  </si>
-  <si>
-    <t>肖继光</t>
-  </si>
-  <si>
-    <t>本周二07/04[35];本周五07/07[35];</t>
-  </si>
-  <si>
-    <t>崔晓洁</t>
-  </si>
-  <si>
-    <t>本周一07/03[25];本周四07/06[31];</t>
+    <t>朱上敏</t>
+  </si>
+  <si>
+    <t>本周三07/05[22];</t>
+  </si>
+  <si>
+    <t>下周一07/10[35];下周三07/12[35];</t>
+  </si>
+  <si>
+    <t>内分泌科门诊</t>
+  </si>
+  <si>
+    <t>冯尤健</t>
+  </si>
+  <si>
+    <t>本周四07/06[40];</t>
+  </si>
+  <si>
+    <t>下周一07/10[42];</t>
+  </si>
+  <si>
+    <t>刘汉昌</t>
+  </si>
+  <si>
+    <t>本周四07/06[33];</t>
+  </si>
+  <si>
+    <t>外科门诊</t>
+  </si>
+  <si>
+    <t>张宪国</t>
+  </si>
+  <si>
+    <t>本周五07/07[34];</t>
+  </si>
+  <si>
+    <t>洪海填</t>
+  </si>
+  <si>
+    <t>产科门诊</t>
+  </si>
+  <si>
+    <t>张金香</t>
+  </si>
+  <si>
+    <t>下周一07/10[26];</t>
+  </si>
+  <si>
+    <t>眼科门诊</t>
+  </si>
+  <si>
+    <t>陈胡挪</t>
+  </si>
+  <si>
+    <t>池晓蓉</t>
+  </si>
+  <si>
+    <t>本周五07/07[31];</t>
+  </si>
+  <si>
+    <t>洪山</t>
   </si>
   <si>
     <t>下周一07/10[30];</t>
   </si>
   <si>
-    <t>消化内科门诊</t>
-  </si>
-  <si>
-    <t>周东生</t>
-  </si>
-  <si>
-    <t>本周四07/06[35];</t>
-  </si>
-  <si>
-    <t>下周一07/10[43];</t>
-  </si>
-  <si>
-    <t>外科门诊</t>
-  </si>
-  <si>
-    <t>张宪国</t>
-  </si>
-  <si>
-    <t>本周五07/07[35];</t>
-  </si>
-  <si>
-    <t>骨二科门诊</t>
-  </si>
-  <si>
-    <t>陆凌云</t>
-  </si>
-  <si>
-    <t>本周一07/03[30];</t>
-  </si>
-  <si>
-    <t>下周一07/10[65];</t>
-  </si>
-  <si>
-    <t>内分泌科门诊</t>
-  </si>
-  <si>
-    <t>冯尤健</t>
-  </si>
-  <si>
-    <t>本周四07/06[42];</t>
-  </si>
-  <si>
-    <t>下周一07/10[42];</t>
-  </si>
-  <si>
     <t>骨一科门诊</t>
   </si>
   <si>
     <t>陈学飞</t>
   </si>
   <si>
-    <t>刘汉昌</t>
-  </si>
-  <si>
-    <t>本周四07/06[34];</t>
-  </si>
-  <si>
     <t>舒诗军</t>
   </si>
   <si>
-    <t>本周六07/08[35];</t>
-  </si>
-  <si>
-    <t>池晓蓉</t>
-  </si>
-  <si>
-    <t>本周五07/07[34];</t>
-  </si>
-  <si>
-    <t>耳鼻喉科门诊</t>
-  </si>
-  <si>
-    <t>刘海楼</t>
+    <t>神经内科门诊</t>
+  </si>
+  <si>
+    <t>张辉</t>
   </si>
   <si>
     <t>姜敏</t>
@@ -156,49 +204,49 @@
     <t>陈魁夫</t>
   </si>
   <si>
-    <t>本周六07/08[35];本周三07/05[34];</t>
-  </si>
-  <si>
-    <t>洪海填</t>
-  </si>
-  <si>
-    <t>本周五07/07[35];本周二07/04[35];</t>
-  </si>
-  <si>
-    <t>朱上敏</t>
-  </si>
-  <si>
-    <t>本周三07/05[35];</t>
-  </si>
-  <si>
-    <t>产科门诊</t>
-  </si>
-  <si>
-    <t>张金香</t>
-  </si>
-  <si>
-    <t>本周一07/03[0];</t>
-  </si>
-  <si>
-    <t>下周一07/10[27];</t>
-  </si>
-  <si>
-    <t>眼科门诊</t>
-  </si>
-  <si>
-    <t>陈胡挪</t>
+    <t>本周六07/08[35];本周三07/05[21];</t>
+  </si>
+  <si>
+    <t>下周三07/12[35];</t>
+  </si>
+  <si>
+    <t>梁富龙</t>
+  </si>
+  <si>
+    <t>陈永春</t>
+  </si>
+  <si>
+    <t>吴谨准</t>
+  </si>
+  <si>
+    <t>下周二07/11[16];</t>
+  </si>
+  <si>
+    <t>呼吸内科门诊</t>
+  </si>
+  <si>
+    <t>邹良能</t>
+  </si>
+  <si>
+    <t>本周三07/05[24];</t>
   </si>
   <si>
     <t>李春阳</t>
   </si>
   <si>
-    <t>本周六07/08[35];本周四07/06[35];</t>
-  </si>
-  <si>
-    <t>洪山</t>
-  </si>
-  <si>
-    <t>本周一07/03[27];本周四07/06[35];</t>
+    <t>本周四07/06[35];本周六07/08[34];</t>
+  </si>
+  <si>
+    <t>肾病风湿免疫科门诊</t>
+  </si>
+  <si>
+    <t>林鹰</t>
+  </si>
+  <si>
+    <t>张燕</t>
+  </si>
+  <si>
+    <t>本周三07/05[13];</t>
   </si>
   <si>
     <t>心血管内科门诊</t>
@@ -210,145 +258,145 @@
     <t>本周四07/06[64];</t>
   </si>
   <si>
-    <t>神经内科门诊</t>
-  </si>
-  <si>
-    <t>张辉</t>
-  </si>
-  <si>
-    <t>梁富龙</t>
-  </si>
-  <si>
-    <t>吴谨准</t>
-  </si>
-  <si>
-    <t>本周二07/04[6];</t>
-  </si>
-  <si>
     <t>中医科门诊</t>
   </si>
   <si>
     <t>苏炳伟</t>
   </si>
   <si>
-    <t>本周六07/08[35];本周二07/04[35];</t>
-  </si>
-  <si>
-    <t>张燕</t>
+    <t>盛群英</t>
+  </si>
+  <si>
+    <t>本周五07/07[30];本周三07/05[26];</t>
+  </si>
+  <si>
+    <t>下周三07/12[30];</t>
+  </si>
+  <si>
+    <t>万会来</t>
+  </si>
+  <si>
+    <t>下周二07/11[65];</t>
+  </si>
+  <si>
+    <t>战晟</t>
+  </si>
+  <si>
+    <t>感染性疾病科门诊</t>
+  </si>
+  <si>
+    <t>薛秀兰</t>
+  </si>
+  <si>
+    <t>下周二07/11[30];</t>
+  </si>
+  <si>
+    <t>钟鸿斌</t>
+  </si>
+  <si>
+    <t>本周五07/07[35];本周三07/05[25];</t>
+  </si>
+  <si>
+    <t>傅翔</t>
+  </si>
+  <si>
+    <t>胸心外科门诊</t>
+  </si>
+  <si>
+    <t>贾平</t>
+  </si>
+  <si>
+    <t>康复医学科门诊</t>
+  </si>
+  <si>
+    <t>李泰标</t>
+  </si>
+  <si>
+    <t>心血管内科专家门诊</t>
+  </si>
+  <si>
+    <t>谢强</t>
+  </si>
+  <si>
+    <t>风湿免疫科门诊</t>
+  </si>
+  <si>
+    <t>肿瘤内科门诊</t>
+  </si>
+  <si>
+    <t>傅鉴乾</t>
+  </si>
+  <si>
+    <t>郑丁炤</t>
+  </si>
+  <si>
+    <t>本周三07/05[25];</t>
+  </si>
+  <si>
+    <t>下周三07/12[35];下周一07/10[35];</t>
+  </si>
+  <si>
+    <t>全科医学科门诊</t>
+  </si>
+  <si>
+    <t>张芸</t>
+  </si>
+  <si>
+    <t>心血管外科专家门诊</t>
+  </si>
+  <si>
+    <t>林乌拉</t>
+  </si>
+  <si>
+    <t>本周六07/08[30];</t>
+  </si>
+  <si>
+    <t>神经外科门诊</t>
+  </si>
+  <si>
+    <t>潘凡</t>
+  </si>
+  <si>
+    <t>白海涛</t>
   </si>
   <si>
     <t>本周三07/05[18];</t>
   </si>
   <si>
-    <t>战晟</t>
-  </si>
-  <si>
-    <t>呼吸内科门诊</t>
-  </si>
-  <si>
-    <t>邹良能</t>
-  </si>
-  <si>
-    <t>肾病风湿免疫科门诊</t>
-  </si>
-  <si>
-    <t>林鹰</t>
-  </si>
-  <si>
-    <t>盛群英</t>
-  </si>
-  <si>
-    <t>本周五07/07[30];本周三07/05[27];</t>
-  </si>
-  <si>
-    <t>钟鸿斌</t>
-  </si>
-  <si>
-    <t>本周三07/05[35];本周五07/07[35];</t>
-  </si>
-  <si>
-    <t>傅翔</t>
-  </si>
-  <si>
-    <t>风湿免疫科门诊</t>
-  </si>
-  <si>
-    <t>本周五07/07[35];本周三07/05[35];</t>
-  </si>
-  <si>
-    <t>心血管内科专家门诊</t>
-  </si>
-  <si>
-    <t>谢强</t>
-  </si>
-  <si>
-    <t>肿瘤内科门诊</t>
-  </si>
-  <si>
-    <t>傅鉴乾</t>
-  </si>
-  <si>
-    <t>感染性疾病科门诊</t>
-  </si>
-  <si>
-    <t>薛秀兰</t>
-  </si>
-  <si>
-    <t>本周二07/04[28];</t>
-  </si>
-  <si>
-    <t>康复医学科门诊</t>
-  </si>
-  <si>
-    <t>郑丁炤</t>
-  </si>
-  <si>
-    <t>胸心外科门诊</t>
-  </si>
-  <si>
-    <t>贾平</t>
-  </si>
-  <si>
-    <t>本周四07/06[35];本周二07/04[35];</t>
-  </si>
-  <si>
-    <t>心血管外科专家门诊</t>
-  </si>
-  <si>
-    <t>林乌拉</t>
-  </si>
-  <si>
-    <t>本周六07/08[30];</t>
-  </si>
-  <si>
-    <t>李泰标</t>
-  </si>
-  <si>
-    <t>陈永春</t>
-  </si>
-  <si>
-    <t>本周二07/04[35];</t>
-  </si>
-  <si>
-    <t>神经外科门诊</t>
+    <t>下周三07/12[20];</t>
   </si>
   <si>
     <t>专家号</t>
   </si>
   <si>
-    <t>本周六07/08[78];本周四07/06[78];本周一07/03[36];本周二07/04[78];本周五07/07[78];本周日07/09[78];本周三07/05[35];</t>
-  </si>
-  <si>
-    <t>下周一07/10[78];</t>
+    <t>本周五07/07[78];本周三07/05[66];本周四07/06[78];本周六07/08[78];本周日07/09[78];</t>
+  </si>
+  <si>
+    <t>下周三07/12[78];下周一07/10[78];下周二07/11[78];</t>
+  </si>
+  <si>
+    <t>本周日07/09[78];本周五07/07[78];本周三07/05[66];本周四07/06[78];本周六07/08[78];</t>
+  </si>
+  <si>
+    <t>朱冰封</t>
   </si>
   <si>
     <t>神经内科</t>
   </si>
   <si>
-    <t>张芸</t>
-  </si>
-  <si>
-    <t>潘凡</t>
+    <t>老年病科</t>
+  </si>
+  <si>
+    <t>陈佳山</t>
+  </si>
+  <si>
+    <t>下周二07/11[35];下周三07/12[35];</t>
+  </si>
+  <si>
+    <t>邱明辉</t>
+  </si>
+  <si>
+    <t>曹本福</t>
   </si>
   <si>
     <t>计划生育门诊</t>
@@ -357,40 +405,34 @@
     <t>普通号</t>
   </si>
   <si>
-    <t>本周六07/08[78];本周二07/04[78];本周五07/07[78];本周一07/03[35];本周日07/09[78];本周三07/05[78];本周四07/06[78];</t>
-  </si>
-  <si>
-    <t>全科医学科门诊</t>
-  </si>
-  <si>
-    <t>本周二07/04[78];本周五07/07[78];本周一07/03[35];本周日07/09[78];本周三07/05[78];本周四07/06[78];本周六07/08[78];</t>
-  </si>
-  <si>
-    <t>本周日07/09[78];本周三07/05[78];本周四07/06[78];本周六07/08[78];本周二07/04[78];本周五07/07[78];本周一07/03[35];</t>
-  </si>
-  <si>
-    <t>老年病科</t>
+    <t>本周六07/08[78];本周三07/05[66];本周四07/06[77];本周日07/09[78];本周五07/07[78];</t>
+  </si>
+  <si>
+    <t>下周一07/10[78];下周三07/12[78];下周二07/11[78];</t>
+  </si>
+  <si>
+    <t>本周日07/09[78];本周五07/07[78];本周六07/08[78];本周三07/05[66];本周四07/06[77];</t>
+  </si>
+  <si>
+    <t>下周二07/11[78];下周一07/10[78];下周三07/12[78];</t>
   </si>
   <si>
     <t>介入诊疗科门诊</t>
   </si>
   <si>
-    <t>本周日07/09[78];本周三07/05[35];本周六07/08[78];本周四07/06[78];本周一07/03[36];本周二07/04[78];本周五07/07[78];</t>
-  </si>
-  <si>
-    <t>本周三07/05[78];本周四07/06[78];本周六07/08[78];本周二07/04[78];本周五07/07[78];本周一07/03[35];本周日07/09[78];</t>
-  </si>
-  <si>
-    <t>本周四07/06[78];本周一07/03[36];本周二07/04[78];本周五07/07[78];本周日07/09[78];本周三07/05[35];本周六07/08[78];</t>
-  </si>
-  <si>
-    <t>本周三07/05[35];本周六07/08[78];本周四07/06[78];本周一07/03[36];本周二07/04[78];本周五07/07[78];本周日07/09[78];</t>
-  </si>
-  <si>
-    <t>本周四07/06[78];本周六07/08[78];本周二07/04[78];本周五07/07[78];本周一07/03[35];本周日07/09[78];本周三07/05[78];</t>
-  </si>
-  <si>
-    <t>本周日07/09[78];本周三07/05[78];本周四07/06[78];本周六07/08[78];本周五07/07[78];本周二07/04[78];本周一07/03[35];</t>
+    <t>本周四07/06[77];本周日07/09[78];本周五07/07[78];本周六07/08[78];本周三07/05[66];</t>
+  </si>
+  <si>
+    <t>本周三07/05[66];本周四07/06[78];本周六07/08[78];本周日07/09[78];本周五07/07[78];</t>
+  </si>
+  <si>
+    <t>下周二07/11[78];下周三07/12[78];下周一07/10[78];</t>
+  </si>
+  <si>
+    <t>本周五07/07[78];本周六07/08[78];本周三07/05[66];本周四07/06[77];本周日07/09[78];</t>
+  </si>
+  <si>
+    <t>本周三07/05[66];本周四07/06[77];本周日07/09[78];本周五07/07[78];本周六07/08[78];</t>
   </si>
   <si>
     <t>中医皮肤科</t>
@@ -402,18 +444,9 @@
     <t>皮肤科</t>
   </si>
   <si>
-    <t>朱冰封</t>
-  </si>
-  <si>
     <t>单忠贵</t>
   </si>
   <si>
-    <t>陈佳山</t>
-  </si>
-  <si>
-    <t>本周三07/05[35];本周二07/04[35];</t>
-  </si>
-  <si>
     <t>文鉴立</t>
   </si>
   <si>
@@ -435,28 +468,16 @@
     <t>下周一07/10[6];</t>
   </si>
   <si>
-    <t>白海涛</t>
-  </si>
-  <si>
-    <t>邱明辉</t>
-  </si>
-  <si>
     <t>崔立山</t>
   </si>
   <si>
-    <t>曹本福</t>
-  </si>
-  <si>
-    <t>本周二07/04[65];</t>
+    <t>本周三07/05[23];</t>
   </si>
   <si>
     <t>柳滨</t>
   </si>
   <si>
-    <t>万会来</t>
-  </si>
-  <si>
-    <t>本周二07/04[63];</t>
+    <t>马榕</t>
   </si>
   <si>
     <t>消化内科二科</t>
@@ -835,7 +856,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D95"/>
+  <dimension ref="A1:D96"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -873,1225 +894,1285 @@
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s"/>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="1" t="s"/>
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="1" t="s"/>
+        <v>17</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>25</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="C8" s="1" t="s"/>
       <c r="D8" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="1" t="s"/>
+        <v>38</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" s="1" t="s"/>
+        <v>44</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="1" t="s"/>
+        <v>24</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>37</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="C15" s="1" t="s"/>
       <c r="D15" s="1" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="1" t="s"/>
+        <v>31</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="D17" s="1" t="s"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D18" s="1" t="s"/>
+        <v>17</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>9</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="D19" s="1" t="s"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>54</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D20" s="1" t="s"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>58</v>
+        <v>24</v>
       </c>
       <c r="D22" s="1" t="s"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D24" s="1" t="s"/>
+        <v>24</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="C25" s="1" t="s"/>
       <c r="D25" s="1" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>64</v>
+        <v>11</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D26" s="1" t="s"/>
+      <c r="C26" s="1" t="s"/>
+      <c r="D26" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D27" s="1" t="s"/>
+        <v>70</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D28" s="1" t="s"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D29" s="1" t="s"/>
+        <v>13</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D30" s="1" t="s"/>
+        <v>76</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>9</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="D31" s="1" t="s"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D32" s="1" t="s"/>
+        <v>13</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D33" s="1" t="s"/>
+        <v>83</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D34" s="1" t="s"/>
+        <v>85</v>
+      </c>
+      <c r="C34" s="1" t="s"/>
+      <c r="D34" s="1" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>75</v>
+        <v>26</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>71</v>
+        <v>17</v>
       </c>
       <c r="D35" s="1" t="s"/>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D36" s="1" t="s"/>
+        <v>89</v>
+      </c>
+      <c r="C36" s="1" t="s"/>
+      <c r="D36" s="1" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C37" s="1" t="s"/>
+        <v>91</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="D37" s="1" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D39" s="1" t="s"/>
+        <v>17</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D41" s="1" t="s"/>
+        <v>99</v>
+      </c>
+      <c r="C41" s="1" t="s"/>
+      <c r="D41" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D42" s="1" t="s"/>
+        <v>92</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D43" s="1" t="s"/>
+        <v>17</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>34</v>
+        <v>96</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D44" s="1" t="s"/>
+        <v>104</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>106</v>
+        <v>13</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>107</v>
+        <v>25</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>66</v>
+        <v>107</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D46" s="1" t="s"/>
+        <v>17</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>78</v>
+        <v>109</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>71</v>
+        <v>110</v>
       </c>
       <c r="D47" s="1" t="s"/>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D48" s="1" t="s"/>
+        <v>112</v>
+      </c>
+      <c r="C48" s="1" t="s"/>
+      <c r="D48" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>104</v>
+        <v>11</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>28</v>
+        <v>114</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>29</v>
+        <v>115</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>111</v>
+        <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>107</v>
+        <v>63</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>84</v>
+        <v>121</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>112</v>
+        <v>64</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>116</v>
+        <v>24</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>107</v>
+        <v>25</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>112</v>
+        <v>74</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>115</v>
+        <v>13</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>107</v>
+        <v>25</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>107</v>
+        <v>124</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>118</v>
+        <v>26</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>107</v>
+        <v>63</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>77</v>
+        <v>111</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>116</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="C57" s="1" t="s"/>
       <c r="D57" s="1" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>61</v>
+        <v>127</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>107</v>
+        <v>130</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
-        <v>64</v>
+        <v>106</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>105</v>
+        <v>128</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>107</v>
+        <v>132</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>105</v>
+        <v>128</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>107</v>
+        <v>130</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="s">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>107</v>
+        <v>130</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>116</v>
+        <v>131</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>107</v>
+        <v>130</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="s">
-        <v>19</v>
+        <v>133</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
-        <v>13</v>
+        <v>133</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>107</v>
+        <v>130</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="s">
-        <v>125</v>
+        <v>73</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>107</v>
+        <v>132</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="s">
-        <v>126</v>
+        <v>77</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>107</v>
+        <v>130</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="s">
-        <v>90</v>
+        <v>58</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>107</v>
+        <v>136</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="s">
-        <v>127</v>
+        <v>36</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>116</v>
+        <v>137</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>107</v>
+        <v>130</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="s">
-        <v>10</v>
+        <v>101</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>107</v>
+        <v>130</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>113</v>
+        <v>138</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>107</v>
+        <v>130</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>107</v>
+        <v>132</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="s">
-        <v>51</v>
+        <v>139</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>107</v>
+        <v>130</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="s">
-        <v>4</v>
+        <v>140</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>107</v>
+        <v>130</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>113</v>
+        <v>138</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>107</v>
+        <v>130</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>105</v>
+        <v>128</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>107</v>
+        <v>132</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="s">
-        <v>55</v>
+        <v>141</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>120</v>
+        <v>134</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>107</v>
+        <v>130</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>123</v>
+        <v>137</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>107</v>
+        <v>130</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="s">
-        <v>104</v>
+        <v>26</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>116</v>
+        <v>137</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>107</v>
+        <v>132</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>116</v>
+        <v>137</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>107</v>
+        <v>130</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>128</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D81" s="1" t="s"/>
+        <v>137</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="s">
-        <v>114</v>
+        <v>4</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>83</v>
+        <v>128</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D82" s="1" t="s"/>
+        <v>137</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B83" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C83" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C83" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D83" s="1" t="s"/>
+      <c r="D83" s="1" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="s">
-        <v>117</v>
+        <v>49</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D84" s="1" t="s"/>
+      <c r="D84" s="1" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="s">
-        <v>77</v>
+        <v>29</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>21</v>
+        <v>131</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>9</v>
+        <v>130</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="s">
-        <v>64</v>
+        <v>111</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D86" s="1" t="s"/>
+        <v>137</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="s">
-        <v>86</v>
+        <v>42</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D87" s="1" t="s"/>
+        <v>131</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="s">
-        <v>136</v>
+        <v>94</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>53</v>
+        <v>104</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>138</v>
+        <v>63</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D89" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B89" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D89" s="1" t="s"/>
     </row>
     <row r="90">
       <c r="A90" s="1" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D90" s="1" t="s"/>
+        <v>104</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D91" s="1" t="s"/>
+        <v>146</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="s">
-        <v>104</v>
+        <v>147</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D92" s="1" t="s"/>
+        <v>148</v>
+      </c>
+      <c r="C92" s="1" t="s"/>
+      <c r="D92" s="1" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="s">
-        <v>23</v>
+        <v>111</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D93" s="1" t="s"/>
+        <v>151</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D94" s="1" t="s"/>
+        <v>104</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="s">
-        <v>147</v>
+        <v>49</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D95" s="1" t="s"/>
+        <v>153</v>
+      </c>
+      <c r="C95" s="1" t="s"/>
+      <c r="D95" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D96" s="1" t="s"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>